<commit_message>
Added support for more table types. Added more unit tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/workbooks/TestSet1.xlsx
+++ b/src/test/resources/workbooks/TestSet1.xlsx
@@ -13,8 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="7" r:id="rId1"/>
-    <sheet name="TableAdapter" sheetId="2" r:id="rId2"/>
-    <sheet name="TableAdapter2" sheetId="6" r:id="rId3"/>
+    <sheet name="Grid V1 Simple" sheetId="2" r:id="rId2"/>
+    <sheet name="Grid V1 Complex" sheetId="6" r:id="rId3"/>
+    <sheet name="Grid V2" sheetId="9" r:id="rId4"/>
+    <sheet name="Lookup V1" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>A</t>
   </si>
@@ -136,25 +138,94 @@
     <t>Rows</t>
   </si>
   <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3 - DEATH AND TPD</t>
-  </si>
-  <si>
-    <t>Test3 - INCOME PROTECTION</t>
-  </si>
-  <si>
-    <t>Test3</t>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>grid</t>
+  </si>
+  <si>
+    <t>Grid V1 Complex</t>
+  </si>
+  <si>
+    <t>Grid V1 Simple</t>
+  </si>
+  <si>
+    <t>Lookup V1</t>
+  </si>
+  <si>
+    <t>Grid - Version 1 - Simple</t>
+  </si>
+  <si>
+    <t>Grid - Version 1 - Complex</t>
+  </si>
+  <si>
+    <t>Lookup - Version 1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>D10+M9</t>
+  </si>
+  <si>
+    <t>Subtract</t>
+  </si>
+  <si>
+    <t>D10-M9</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>D10*M9</t>
+  </si>
+  <si>
+    <t>Divide</t>
+  </si>
+  <si>
+    <t>D10/M9</t>
+  </si>
+  <si>
+    <t>Multi-column and Multi-row Table</t>
+  </si>
+  <si>
+    <t>column1</t>
+  </si>
+  <si>
+    <t>column2</t>
+  </si>
+  <si>
+    <t>column3</t>
+  </si>
+  <si>
+    <t>column4</t>
+  </si>
+  <si>
+    <t>row1</t>
+  </si>
+  <si>
+    <t>row2</t>
+  </si>
+  <si>
+    <t>row3</t>
+  </si>
+  <si>
+    <t>Grid V2</t>
+  </si>
+  <si>
+    <t>Grid - Version 2</t>
   </si>
 </sst>
 </file>
@@ -178,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -326,11 +403,246 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,25 +660,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -408,6 +702,153 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I15"/>
+  <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,217 +1139,484 @@
     <col min="2" max="3" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="57"/>
+      <c r="F2" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="I2" s="57"/>
+      <c r="J2" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="J3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="24">
+      <c r="K3" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="18">
         <v>1</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="19">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18">
+        <v>5</v>
+      </c>
+      <c r="G4" s="19">
+        <v>4</v>
+      </c>
+      <c r="H4" s="18">
+        <v>1</v>
+      </c>
+      <c r="I4" s="20">
+        <v>4</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="21">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22">
+        <v>8</v>
+      </c>
+      <c r="F5" s="21">
+        <v>5</v>
+      </c>
+      <c r="G5" s="22">
+        <v>3</v>
+      </c>
+      <c r="H5" s="21">
+        <v>1</v>
+      </c>
+      <c r="I5" s="23">
+        <v>4</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="21">
+        <v>3</v>
+      </c>
+      <c r="E6" s="22">
+        <v>4</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <v>1</v>
+      </c>
+      <c r="I6" s="23">
+        <v>4</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="21">
         <v>2</v>
       </c>
-      <c r="F4" s="24">
-        <v>36</v>
-      </c>
-      <c r="G4" s="25">
-        <v>8</v>
-      </c>
-      <c r="H4" s="24">
-        <v>1</v>
-      </c>
-      <c r="I4" s="26">
+      <c r="E7" s="22">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="F7" s="21">
+        <v>5</v>
+      </c>
+      <c r="G7" s="22">
+        <v>4</v>
+      </c>
+      <c r="H7" s="21">
+        <v>3</v>
+      </c>
+      <c r="I7" s="23">
+        <v>4</v>
+      </c>
+      <c r="J7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="27">
-        <v>1</v>
-      </c>
-      <c r="E5" s="28">
-        <v>1</v>
-      </c>
-      <c r="F5" s="27">
-        <v>5</v>
-      </c>
-      <c r="G5" s="28">
-        <v>4</v>
-      </c>
-      <c r="H5" s="27">
-        <v>1</v>
-      </c>
-      <c r="I5" s="29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="29"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="29"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="17"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="29"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="29"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="17"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="29"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="29"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="29"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="17"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="32"/>
+      <c r="K7" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="11"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="23"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="23"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="11"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="23"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="23"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="11"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="23"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="23"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="23"/>
+    </row>
+    <row r="30" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -919,7 +1627,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:H21"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,11 +1636,11 @@
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
@@ -944,14 +1652,14 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
@@ -963,24 +1671,24 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -1079,7 +1787,7 @@
   <dimension ref="C2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,17 +1806,17 @@
       <c r="C8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="62" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1116,27 +1824,27 @@
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C11" s="6">
@@ -1226,4 +1934,337 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="5" max="5" width="2.5" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+    </row>
+    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="39"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="73"/>
+      <c r="J6" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="41"/>
+      <c r="F7" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="39"/>
+    </row>
+    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="41"/>
+      <c r="F8" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="39"/>
+    </row>
+    <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="39"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="39"/>
+      <c r="B10" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="50">
+        <v>1</v>
+      </c>
+      <c r="E10" s="51"/>
+      <c r="F10" s="28">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19">
+        <v>2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>3</v>
+      </c>
+      <c r="I10" s="19">
+        <v>4</v>
+      </c>
+      <c r="J10" s="27">
+        <v>5</v>
+      </c>
+      <c r="K10" s="39"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="64"/>
+      <c r="D11" s="52">
+        <v>2</v>
+      </c>
+      <c r="E11" s="51"/>
+      <c r="F11" s="29">
+        <v>6</v>
+      </c>
+      <c r="G11" s="22">
+        <v>7</v>
+      </c>
+      <c r="H11" s="21">
+        <v>8</v>
+      </c>
+      <c r="I11" s="22">
+        <v>9</v>
+      </c>
+      <c r="J11" s="23">
+        <v>10</v>
+      </c>
+      <c r="K11" s="39"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="52">
+        <v>3</v>
+      </c>
+      <c r="E12" s="51"/>
+      <c r="F12" s="29">
+        <v>11</v>
+      </c>
+      <c r="G12" s="22">
+        <v>12</v>
+      </c>
+      <c r="H12" s="21">
+        <v>13</v>
+      </c>
+      <c r="I12" s="22">
+        <v>14</v>
+      </c>
+      <c r="J12" s="23">
+        <v>15</v>
+      </c>
+      <c r="K12" s="39"/>
+    </row>
+    <row r="13" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="68"/>
+      <c r="D13" s="54">
+        <v>4</v>
+      </c>
+      <c r="E13" s="51"/>
+      <c r="F13" s="55">
+        <v>16</v>
+      </c>
+      <c r="G13" s="25">
+        <v>17</v>
+      </c>
+      <c r="H13" s="24">
+        <v>18</v>
+      </c>
+      <c r="I13" s="25">
+        <v>19</v>
+      </c>
+      <c r="J13" s="26">
+        <v>20</v>
+      </c>
+      <c r="K13" s="39"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="F8:J8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>